<commit_message>
Plotted Lin Fst vs. Distance
</commit_message>
<xml_diff>
--- a/Pairwise Fst Matrix.xlsx
+++ b/Pairwise Fst Matrix.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrafitz/Documents/GitHub/Premnas-biaculeatus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyras\OneDrive\Documents\GitHub\Premnas-biaculeatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5DA03A3-8568-4206-819F-9401C1A7E5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32180" yWindow="5820" windowWidth="28160" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="34515" yWindow="3525" windowWidth="21210" windowHeight="11835" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All Pop All Loci" sheetId="1" r:id="rId1"/>
+    <sheet name="All Pop No ACHB9" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,15 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="2">
   <si>
     <t>Pop</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -73,6 +86,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -340,16 +356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -360,121 +376,121 @@
         <v>2</v>
       </c>
       <c r="D1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L1">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="M1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>3.395E-3</v>
-      </c>
-      <c r="D2">
-        <v>6.888E-3</v>
-      </c>
-      <c r="E2">
-        <v>7.5599999999999999E-3</v>
-      </c>
-      <c r="F2">
-        <v>1.128E-2</v>
-      </c>
-      <c r="G2">
-        <v>-2.3860000000000001E-3</v>
-      </c>
-      <c r="H2">
-        <v>1.9819999999999998E-3</v>
-      </c>
-      <c r="I2">
-        <v>-1.243E-2</v>
-      </c>
-      <c r="J2">
-        <v>-6.8739999999999999E-3</v>
-      </c>
-      <c r="K2">
-        <v>-3.7929999999999998E-2</v>
-      </c>
-      <c r="L2">
-        <v>1.1310000000000001E-2</v>
-      </c>
-      <c r="M2">
-        <v>3.5140000000000002E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3.395E-3</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>6.2940000000000001E-3</v>
-      </c>
-      <c r="E3">
-        <v>4.8220000000000001E-4</v>
-      </c>
-      <c r="F3">
-        <v>3.8830000000000002E-3</v>
-      </c>
-      <c r="G3">
-        <v>5.1460000000000004E-3</v>
-      </c>
-      <c r="H3">
-        <v>-1.065E-3</v>
-      </c>
-      <c r="I3">
-        <v>-1.129E-2</v>
-      </c>
-      <c r="J3">
-        <v>3.722E-3</v>
-      </c>
-      <c r="K3">
-        <v>-8.3850000000000001E-3</v>
-      </c>
-      <c r="L3">
-        <v>7.4390000000000003E-3</v>
-      </c>
-      <c r="M3">
-        <v>3.3590000000000002E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>6.888E-3</v>
@@ -482,40 +498,40 @@
       <c r="C4">
         <v>6.2940000000000001E-3</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>-7.7200000000000001E-4</v>
-      </c>
-      <c r="F4">
-        <v>1.671E-3</v>
-      </c>
-      <c r="G4">
-        <v>6.2420000000000002E-3</v>
-      </c>
-      <c r="H4">
-        <v>-7.3130000000000005E-4</v>
-      </c>
-      <c r="I4">
-        <v>-3.039E-2</v>
-      </c>
-      <c r="J4">
-        <v>-2.095E-2</v>
-      </c>
-      <c r="K4">
-        <v>-2.0490000000000001E-2</v>
-      </c>
-      <c r="L4">
-        <v>-3.9069999999999999E-3</v>
-      </c>
-      <c r="M4">
-        <v>-2.0650000000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>7.5599999999999999E-3</v>
@@ -526,37 +542,37 @@
       <c r="D5">
         <v>-7.7200000000000001E-4</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>-2.062E-3</v>
-      </c>
-      <c r="G5">
-        <v>1.292E-3</v>
-      </c>
-      <c r="H5">
-        <v>-7.8359999999999992E-3</v>
-      </c>
-      <c r="I5">
-        <v>-2.5430000000000001E-2</v>
-      </c>
-      <c r="J5">
-        <v>6.96E-3</v>
-      </c>
-      <c r="K5">
-        <v>-1.018E-2</v>
-      </c>
-      <c r="L5">
-        <v>-8.9599999999999992E-3</v>
-      </c>
-      <c r="M5">
-        <v>4.9319999999999998E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1.128E-2</v>
@@ -570,34 +586,34 @@
       <c r="E6">
         <v>-2.062E-3</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>-2.6069999999999999E-3</v>
-      </c>
-      <c r="H6">
-        <v>1.784E-4</v>
-      </c>
-      <c r="I6">
-        <v>-2.0580000000000001E-2</v>
-      </c>
-      <c r="J6">
-        <v>-3.5999999999999997E-2</v>
-      </c>
-      <c r="K6">
-        <v>-2.8389999999999999E-2</v>
-      </c>
-      <c r="L6">
-        <v>6.8939999999999995E-4</v>
-      </c>
-      <c r="M6">
-        <v>5.0179999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>-2.3860000000000001E-3</v>
@@ -614,31 +630,31 @@
       <c r="F7">
         <v>-2.6069999999999999E-3</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>-6.8500000000000002E-3</v>
-      </c>
-      <c r="I7">
-        <v>-2.7869999999999999E-2</v>
-      </c>
-      <c r="J7">
-        <v>-1.4370000000000001E-2</v>
-      </c>
-      <c r="K7">
-        <v>-3.449E-2</v>
-      </c>
-      <c r="L7">
-        <v>5.2370000000000003E-3</v>
-      </c>
-      <c r="M7">
-        <v>4.6719999999999999E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1.9819999999999998E-3</v>
@@ -658,28 +674,28 @@
       <c r="G8">
         <v>-6.8500000000000002E-3</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>-3.449E-2</v>
-      </c>
-      <c r="J8">
-        <v>-3.175E-2</v>
-      </c>
-      <c r="K8">
-        <v>-5.2040000000000003E-2</v>
-      </c>
-      <c r="L8">
-        <v>5.9899999999999997E-3</v>
-      </c>
-      <c r="M8">
-        <v>5.4450000000000002E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>-1.243E-2</v>
@@ -702,25 +718,25 @@
       <c r="H9">
         <v>-3.449E-2</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>-8.0430000000000001E-2</v>
-      </c>
-      <c r="K9">
-        <v>-3.8760000000000003E-2</v>
-      </c>
-      <c r="L9">
-        <v>-2.341E-2</v>
-      </c>
-      <c r="M9">
-        <v>-7.9339999999999999E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>-6.8739999999999999E-3</v>
@@ -746,22 +762,22 @@
       <c r="I10">
         <v>-8.0430000000000001E-2</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>-0.2029</v>
-      </c>
-      <c r="L10">
-        <v>-4.9100000000000003E-3</v>
-      </c>
-      <c r="M10">
-        <v>-4.3860000000000001E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>-3.7929999999999998E-2</v>
@@ -790,19 +806,19 @@
       <c r="J11">
         <v>-0.2029</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>3.356E-2</v>
-      </c>
-      <c r="M11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>1.1310000000000001E-2</v>
@@ -834,16 +850,16 @@
       <c r="K12">
         <v>3.356E-2</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>-2.435E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>3.5140000000000002E-3</v>
@@ -878,8 +894,569 @@
       <c r="L13">
         <v>-2.435E-2</v>
       </c>
-      <c r="M13">
+      <c r="M13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3722B2BB-8EC6-49E0-B1F5-A7E853D4198F}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.09765625" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" customWidth="1"/>
+    <col min="5" max="5" width="12.69921875" customWidth="1"/>
+    <col min="6" max="6" width="11.296875" customWidth="1"/>
+    <col min="7" max="7" width="11.09765625" customWidth="1"/>
+    <col min="8" max="8" width="11.8984375" customWidth="1"/>
+    <col min="9" max="9" width="11.09765625" customWidth="1"/>
+    <col min="10" max="10" width="12.09765625" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" customWidth="1"/>
+    <col min="12" max="13" width="11.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>11</v>
+      </c>
+      <c r="I1">
+        <v>13</v>
+      </c>
+      <c r="J1">
+        <v>14</v>
+      </c>
+      <c r="K1">
+        <v>15</v>
+      </c>
+      <c r="L1">
+        <v>19</v>
+      </c>
+      <c r="M1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.9970000000000001E-3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>4.8300000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.7009999999999999E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>6.6709999999999998E-3</v>
+      </c>
+      <c r="C5">
+        <v>1.152E-3</v>
+      </c>
+      <c r="D5">
+        <v>4.3540000000000001E-4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1.289E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.1020000000000001E-3</v>
+      </c>
+      <c r="D6">
+        <v>3.5409999999999999E-3</v>
+      </c>
+      <c r="E6">
+        <v>-2.2680000000000001E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>-3.5500000000000002E-3</v>
+      </c>
+      <c r="C7">
+        <v>1.946E-3</v>
+      </c>
+      <c r="D7">
+        <v>7.2680000000000002E-3</v>
+      </c>
+      <c r="E7">
+        <v>9.3380000000000004E-4</v>
+      </c>
+      <c r="F7">
+        <v>-1.23E-3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1.077E-3</v>
+      </c>
+      <c r="C8">
+        <v>-2.4069999999999999E-3</v>
+      </c>
+      <c r="D8">
+        <v>-6.1450000000000003E-4</v>
+      </c>
+      <c r="E8">
+        <v>-7.62E-3</v>
+      </c>
+      <c r="F8">
+        <v>1.8779999999999999E-3</v>
+      </c>
+      <c r="G8">
+        <v>-6.136E-3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>-1.37E-2</v>
+      </c>
+      <c r="C9">
+        <v>-1.6410000000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>-2.827E-2</v>
+      </c>
+      <c r="E9">
+        <v>-2.3820000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>-1.6330000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>-2.545E-2</v>
+      </c>
+      <c r="H9">
+        <v>-3.0630000000000001E-2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>-1.1310000000000001E-3</v>
+      </c>
+      <c r="C10">
+        <v>2.911E-3</v>
+      </c>
+      <c r="D10">
+        <v>-1.4959999999999999E-2</v>
+      </c>
+      <c r="E10">
+        <v>1.226E-2</v>
+      </c>
+      <c r="F10">
+        <v>-2.826E-2</v>
+      </c>
+      <c r="G10">
+        <v>-1.3169999999999999E-2</v>
+      </c>
+      <c r="H10">
+        <v>-2.8750000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>-7.1419999999999997E-2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>-7.2249999999999995E-2</v>
+      </c>
+      <c r="C11">
+        <v>-2.9790000000000001E-2</v>
+      </c>
+      <c r="D11">
+        <v>-2.674E-2</v>
+      </c>
+      <c r="E11">
+        <v>-1.634E-2</v>
+      </c>
+      <c r="F11">
+        <v>-4.684E-2</v>
+      </c>
+      <c r="G11">
+        <v>-6.4519999999999994E-2</v>
+      </c>
+      <c r="H11">
+        <v>-7.6069999999999999E-2</v>
+      </c>
+      <c r="I11">
+        <v>-5.5160000000000001E-2</v>
+      </c>
+      <c r="J11">
+        <v>-0.2074</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>1.171E-2</v>
+      </c>
+      <c r="C12">
+        <v>6.2880000000000002E-3</v>
+      </c>
+      <c r="D12">
+        <v>-3.2469999999999999E-3</v>
+      </c>
+      <c r="E12">
+        <v>-8.2629999999999995E-3</v>
+      </c>
+      <c r="F12">
+        <v>2.7820000000000002E-3</v>
+      </c>
+      <c r="G12">
+        <v>7.084E-3</v>
+      </c>
+      <c r="H12">
+        <v>8.7819999999999999E-3</v>
+      </c>
+      <c r="I12">
+        <v>-1.874E-2</v>
+      </c>
+      <c r="J12">
+        <v>1.598E-3</v>
+      </c>
+      <c r="K12">
+        <v>1.9179999999999999E-2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>-7.5249999999999996E-3</v>
+      </c>
+      <c r="C13">
+        <v>2.2110000000000001E-2</v>
+      </c>
+      <c r="D13">
+        <v>-2.324E-2</v>
+      </c>
+      <c r="E13">
+        <v>1.286E-3</v>
+      </c>
+      <c r="F13">
+        <v>3.8930000000000002E-3</v>
+      </c>
+      <c r="G13">
+        <v>4.9370000000000004E-3</v>
+      </c>
+      <c r="H13">
+        <v>7.5900000000000004E-3</v>
+      </c>
+      <c r="I13">
+        <v>6.0819999999999997E-3</v>
+      </c>
+      <c r="J13">
+        <v>-1.217E-2</v>
+      </c>
+      <c r="K13">
+        <v>8.1820000000000004E-2</v>
+      </c>
+      <c r="L13">
+        <v>-3.006E-2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excluded pop 19 for plotting lin fst vs. distance
</commit_message>
<xml_diff>
--- a/Pairwise Fst Matrix.xlsx
+++ b/Pairwise Fst Matrix.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyras\OneDrive\Documents\GitHub\Premnas-biaculeatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5DA03A3-8568-4206-819F-9401C1A7E5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D453A7E8-C244-498A-877C-3162A0FA94FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34515" yWindow="3525" windowWidth="21210" windowHeight="11835" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32730" yWindow="2550" windowWidth="24150" windowHeight="12915" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Pop All Loci" sheetId="1" r:id="rId1"/>
     <sheet name="All Pop No ACHB9" sheetId="2" r:id="rId2"/>
+    <sheet name="No 19 No ACHB9" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="2">
   <si>
     <t>Pop</t>
   </si>
@@ -359,8 +360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:M13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -907,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3722B2BB-8EC6-49E0-B1F5-A7E853D4198F}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1462,4 +1463,487 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19DCBCF-E7D5-4800-AC00-F928E2535BA7}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" customWidth="1"/>
+    <col min="6" max="6" width="11.09765625" customWidth="1"/>
+    <col min="7" max="7" width="11.8984375" customWidth="1"/>
+    <col min="8" max="8" width="11.796875" customWidth="1"/>
+    <col min="9" max="9" width="11.09765625" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" customWidth="1"/>
+    <col min="11" max="11" width="10.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>11</v>
+      </c>
+      <c r="I1">
+        <v>13</v>
+      </c>
+      <c r="J1">
+        <v>14</v>
+      </c>
+      <c r="K1">
+        <v>15</v>
+      </c>
+      <c r="L1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.9970000000000001E-3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>4.8300000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.7009999999999999E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>6.6709999999999998E-3</v>
+      </c>
+      <c r="C5">
+        <v>1.152E-3</v>
+      </c>
+      <c r="D5">
+        <v>4.3540000000000001E-4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1.289E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.1020000000000001E-3</v>
+      </c>
+      <c r="D6">
+        <v>3.5409999999999999E-3</v>
+      </c>
+      <c r="E6">
+        <v>-2.2680000000000001E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>-3.5500000000000002E-3</v>
+      </c>
+      <c r="C7">
+        <v>1.946E-3</v>
+      </c>
+      <c r="D7">
+        <v>7.2680000000000002E-3</v>
+      </c>
+      <c r="E7">
+        <v>9.3380000000000004E-4</v>
+      </c>
+      <c r="F7">
+        <v>-1.23E-3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1.077E-3</v>
+      </c>
+      <c r="C8">
+        <v>-2.4069999999999999E-3</v>
+      </c>
+      <c r="D8">
+        <v>-6.1450000000000003E-4</v>
+      </c>
+      <c r="E8">
+        <v>-7.62E-3</v>
+      </c>
+      <c r="F8">
+        <v>1.8779999999999999E-3</v>
+      </c>
+      <c r="G8">
+        <v>-6.136E-3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>-1.37E-2</v>
+      </c>
+      <c r="C9">
+        <v>-1.6410000000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>-2.827E-2</v>
+      </c>
+      <c r="E9">
+        <v>-2.3820000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>-1.6330000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>-2.545E-2</v>
+      </c>
+      <c r="H9">
+        <v>-3.0630000000000001E-2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>-1.1310000000000001E-3</v>
+      </c>
+      <c r="C10">
+        <v>2.911E-3</v>
+      </c>
+      <c r="D10">
+        <v>-1.4959999999999999E-2</v>
+      </c>
+      <c r="E10">
+        <v>1.226E-2</v>
+      </c>
+      <c r="F10">
+        <v>-2.826E-2</v>
+      </c>
+      <c r="G10">
+        <v>-1.3169999999999999E-2</v>
+      </c>
+      <c r="H10">
+        <v>-2.8750000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>-7.1419999999999997E-2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>-7.2249999999999995E-2</v>
+      </c>
+      <c r="C11">
+        <v>-2.9790000000000001E-2</v>
+      </c>
+      <c r="D11">
+        <v>-2.674E-2</v>
+      </c>
+      <c r="E11">
+        <v>-1.634E-2</v>
+      </c>
+      <c r="F11">
+        <v>-4.684E-2</v>
+      </c>
+      <c r="G11">
+        <v>-6.4519999999999994E-2</v>
+      </c>
+      <c r="H11">
+        <v>-7.6069999999999999E-2</v>
+      </c>
+      <c r="I11">
+        <v>-5.5160000000000001E-2</v>
+      </c>
+      <c r="J11">
+        <v>-0.2074</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>-7.5249999999999996E-3</v>
+      </c>
+      <c r="C12">
+        <v>2.2110000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>-2.324E-2</v>
+      </c>
+      <c r="E12">
+        <v>1.286E-3</v>
+      </c>
+      <c r="F12">
+        <v>3.8930000000000002E-3</v>
+      </c>
+      <c r="G12">
+        <v>4.9370000000000004E-3</v>
+      </c>
+      <c r="H12">
+        <v>7.5900000000000004E-3</v>
+      </c>
+      <c r="I12">
+        <v>6.0819999999999997E-3</v>
+      </c>
+      <c r="J12">
+        <v>-1.217E-2</v>
+      </c>
+      <c r="K12">
+        <v>8.1820000000000004E-2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>